<commit_message>
Uppdatering av Excelfiler och infogat bild
</commit_message>
<xml_diff>
--- a/docs/Kartläggning_community.xlsx
+++ b/docs/Kartläggning_community.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clarala/DIDsteg2/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97EE94F9-5B13-E247-8F9C-05E6FEB7C00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B8DA8A-F4BB-B241-9E26-9096044707BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="500" windowWidth="28240" windowHeight="16020" xr2:uid="{7BC09E43-1041-714B-B107-1A982B11F32C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kartläggande frågor" sheetId="1" r:id="rId1"/>
+    <sheet name="Sammanfattning Övergripande" sheetId="2" r:id="rId1"/>
+    <sheet name="Kartläggande frågor" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
     <t>Datum</t>
   </si>
@@ -79,9 +80,6 @@
     </r>
   </si>
   <si>
-    <t>Kartläggning Basutbud TRYGGT NÄRSAMHÄLLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Det finns samverkansformer för att bedriva områdesarbete mellan kommunala verksamheter, myndigheter, bostadsbolag, civilsamhällesorganisationer, näringsliv, hälso- och sjukvård samt invånare i området. </t>
   </si>
   <si>
@@ -155,13 +153,34 @@
   </si>
   <si>
     <t>Barn och unga involveras i planeringen och genomförandet av organiserade aktiviteter.</t>
+  </si>
+  <si>
+    <t>Denna kartläggning besvaras av kommun:</t>
+  </si>
+  <si>
+    <t>SAMMANFATTNING</t>
+  </si>
+  <si>
+    <t>26-XX-XX</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>Nej</t>
+  </si>
+  <si>
+    <t>Kartläggning TRYGGT NÄRSAMHÄLLE</t>
+  </si>
+  <si>
+    <t>Kryssa i de påståenden som stämmer för er kommun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -200,6 +219,26 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF242424"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,7 +248,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -355,11 +394,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -414,20 +464,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -447,6 +512,61 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Bildobjekt 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3651594-0F24-794E-AB28-F514E16F9C60}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5397500" y="38100"/>
+          <a:ext cx="1752600" cy="879475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -817,10 +937,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CC34EE-B55D-6C4C-A07E-2F5F91D32621}">
-  <dimension ref="A1:G32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34ED2ECD-D63C-A64A-9AB6-FAC530F8DCE1}">
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="50.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="19">
+      <c r="A1" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="20">
+      <c r="A3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="32" customFormat="1" ht="18" thickBot="1">
+      <c r="A8" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:6" ht="101" thickTop="1">
+      <c r="A9" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="40">
+      <c r="A10" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" ht="40">
+      <c r="A11" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" ht="20">
+      <c r="A12" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="14" spans="1:6" ht="20">
+      <c r="A14" s="33" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="20">
+      <c r="A15" s="33" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:XFD12" xr:uid="{E14352AD-EE47-0D4B-B55B-F0F36797FD44}">
+      <formula1>$A$14:$A$15</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4CC34EE-B55D-6C4C-A07E-2F5F91D32621}">
+  <dimension ref="A1:G33"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -829,7 +1058,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19">
       <c r="A1" s="13" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="20">
@@ -840,60 +1069,54 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19">
-      <c r="A4" s="14"/>
-    </row>
-    <row r="5" spans="1:7" s="20" customFormat="1" ht="18" thickBot="1">
-      <c r="A5" s="18" t="s">
+    <row r="4" spans="1:7" ht="17">
+      <c r="A4" s="34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="34"/>
+    </row>
+    <row r="6" spans="1:7" s="20" customFormat="1" ht="18" thickBot="1">
+      <c r="A6" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="C6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D6" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:7" ht="45" thickTop="1">
-      <c r="A6" s="12" t="s">
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:7" ht="65" thickTop="1">
+      <c r="A7" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="17"/>
-    </row>
-    <row r="7" spans="1:7" s="11" customFormat="1" ht="100">
-      <c r="A7" s="15" t="s">
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="1:7" s="11" customFormat="1" ht="100">
+      <c r="A8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" s="11" customFormat="1" ht="40">
+      <c r="A9" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" s="11" customFormat="1" ht="40">
-      <c r="A8" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" s="11" customFormat="1" ht="60">
-      <c r="A9" s="15" t="s">
-        <v>10</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="10"/>
@@ -902,11 +1125,11 @@
       <c r="F9" s="9"/>
       <c r="G9" s="9"/>
     </row>
-    <row r="10" spans="1:7" s="11" customFormat="1" ht="40">
+    <row r="10" spans="1:7" s="11" customFormat="1" ht="60">
       <c r="A10" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="10"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -915,7 +1138,7 @@
     </row>
     <row r="11" spans="1:7" s="11" customFormat="1" ht="40">
       <c r="A11" s="15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
@@ -924,53 +1147,53 @@
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" ht="50" customHeight="1">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:7" s="11" customFormat="1" ht="40">
+      <c r="A12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="1:7" s="6" customFormat="1" ht="50" customHeight="1">
+      <c r="A13" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" s="11" customFormat="1" ht="40">
+      <c r="A14" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="28"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" s="11" customFormat="1" ht="40">
-      <c r="A13" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="1:7" s="11" customFormat="1" ht="60">
-      <c r="A14" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
       <c r="F14" s="9"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="1:7" s="4" customFormat="1" ht="40">
-      <c r="A15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
+    <row r="15" spans="1:7" s="11" customFormat="1" ht="60">
+      <c r="A15" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" ht="40">
       <c r="A16" s="16" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -979,9 +1202,9 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="60">
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="40">
       <c r="A17" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -990,53 +1213,53 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" s="6" customFormat="1" ht="50" customHeight="1">
-      <c r="A18" s="22" t="s">
+    <row r="18" spans="1:7" s="4" customFormat="1" ht="60">
+      <c r="A18" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" s="6" customFormat="1" ht="50" customHeight="1">
+      <c r="A19" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="25"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
+    </row>
+    <row r="20" spans="1:7" s="11" customFormat="1" ht="40">
+      <c r="A20" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="28"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-    </row>
-    <row r="19" spans="1:7" s="11" customFormat="1" ht="40">
-      <c r="A19" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-    </row>
-    <row r="20" spans="1:7" s="11" customFormat="1" ht="60">
-      <c r="A20" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
       <c r="F20" s="9"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" s="4" customFormat="1" ht="40">
-      <c r="A21" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-    </row>
-    <row r="22" spans="1:7" s="4" customFormat="1" ht="80">
+    <row r="21" spans="1:7" s="11" customFormat="1" ht="60">
+      <c r="A21" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="10"/>
+      <c r="C21" s="10"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+    </row>
+    <row r="22" spans="1:7" s="4" customFormat="1" ht="40">
       <c r="A22" s="16" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1045,9 +1268,9 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="60">
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="80">
       <c r="A23" s="16" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1056,7 +1279,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="40">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="60">
       <c r="A24" s="16" t="s">
         <v>24</v>
       </c>
@@ -1067,94 +1290,105 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7">
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:7" ht="22">
-      <c r="A26" s="21" t="s">
+    <row r="25" spans="1:7" s="4" customFormat="1" ht="40">
+      <c r="A25" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" ht="22">
+      <c r="A27" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+    </row>
+    <row r="28" spans="1:7" s="11" customFormat="1" ht="20">
+      <c r="A28" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:7" s="11" customFormat="1" ht="20">
-      <c r="A27" s="15" t="s">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
+    </row>
+    <row r="29" spans="1:7" s="4" customFormat="1" ht="98" customHeight="1">
+      <c r="A29" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="B27" s="27"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-    </row>
-    <row r="28" spans="1:7" s="4" customFormat="1" ht="98" customHeight="1">
-      <c r="A28" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="60">
-      <c r="A29" s="16" t="s">
-        <v>29</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="40">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="60">
       <c r="A30" s="16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" ht="20">
+    <row r="31" spans="1:7" s="4" customFormat="1" ht="40">
       <c r="A31" s="16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="40">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="20">
       <c r="A32" s="16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
     </row>
+    <row r="33" spans="1:5" s="4" customFormat="1" ht="40">
+      <c r="A33" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D6:D7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="F6:F7"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="B19:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>